<commit_message>
Enable ZEV stds for nonroad vehicles
</commit_message>
<xml_diff>
--- a/InputData/trans/VSbS/Vehicle Shares by Subregion.xlsx
+++ b/InputData/trans/VSbS/Vehicle Shares by Subregion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\trans\VSbS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\VSbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7C4D67-74A1-4BF9-A001-F474636F2E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E91793-1818-4D44-889A-A4ABF3FC1BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16440" yWindow="2445" windowWidth="29940" windowHeight="20805" xr2:uid="{F34BB550-7D2B-439D-9C81-D72ED5B29ABD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F34BB550-7D2B-439D-9C81-D72ED5B29ABD}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1075,7 +1075,7 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="37" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -1244,6 +1244,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1274,11 +1276,6 @@
     <xf numFmtId="37" fontId="5" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma 2" xfId="5" xr:uid="{7B2DBB66-964B-4992-8A85-CF7563C0181E}"/>
@@ -1289,147 +1286,7 @@
     <cellStyle name="Normal 5" xfId="6" xr:uid="{58A5829F-0798-4AC5-A887-3CBCA8BB0153}"/>
     <cellStyle name="Normal 8 2" xfId="4" xr:uid="{1E08BF75-563B-4006-9FB0-94126509CFF1}"/>
   </cellStyles>
-  <dxfs count="34">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1818,26 +1675,23 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="112" t="s">
+      <c r="A10" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="112" t="s">
+      <c r="A11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="112"/>
-    </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="113" t="s">
+      <c r="A13" s="102" t="s">
         <v>107</v>
       </c>
-      <c r="B13" s="114"/>
-    </row>
-    <row r="14" spans="1:2" s="116" customFormat="1">
-      <c r="A14" s="115"/>
+      <c r="B13" s="103"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1"/>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
@@ -1910,24 +1764,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="103"/>
-      <c r="O1" s="103"/>
-      <c r="P1" s="103"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="98"/>
@@ -1971,51 +1825,51 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="94"/>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="105"/>
-      <c r="M4" s="105"/>
-      <c r="N4" s="105"/>
-      <c r="O4" s="105"/>
-      <c r="P4" s="106"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="107"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="107"/>
+      <c r="I4" s="107"/>
+      <c r="J4" s="107"/>
+      <c r="K4" s="107"/>
+      <c r="L4" s="107"/>
+      <c r="M4" s="107"/>
+      <c r="N4" s="107"/>
+      <c r="O4" s="107"/>
+      <c r="P4" s="108"/>
     </row>
     <row r="5" spans="1:16" ht="9">
       <c r="A5" s="79"/>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="109" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="109" t="s">
+      <c r="C5" s="110"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="111" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="108"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="108" t="s">
+      <c r="F5" s="110"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="110" t="s">
         <v>71</v>
       </c>
-      <c r="I5" s="108"/>
-      <c r="J5" s="108"/>
-      <c r="K5" s="109" t="s">
+      <c r="I5" s="110"/>
+      <c r="J5" s="110"/>
+      <c r="K5" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="L5" s="108"/>
-      <c r="M5" s="110"/>
-      <c r="N5" s="108" t="s">
+      <c r="L5" s="110"/>
+      <c r="M5" s="112"/>
+      <c r="N5" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="O5" s="108"/>
-      <c r="P5" s="111"/>
+      <c r="O5" s="110"/>
+      <c r="P5" s="113"/>
     </row>
     <row r="6" spans="1:16" ht="9">
       <c r="A6" s="79" t="s">
@@ -4798,24 +4652,24 @@
       <c r="P62" s="5"/>
     </row>
     <row r="63" spans="1:16" ht="39.6" customHeight="1">
-      <c r="A63" s="102" t="s">
+      <c r="A63" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="B63" s="102"/>
-      <c r="C63" s="102"/>
-      <c r="D63" s="102"/>
-      <c r="E63" s="102"/>
-      <c r="F63" s="102"/>
-      <c r="G63" s="102"/>
-      <c r="H63" s="102"/>
-      <c r="I63" s="102"/>
-      <c r="J63" s="102"/>
-      <c r="K63" s="102"/>
-      <c r="L63" s="102"/>
-      <c r="M63" s="102"/>
-      <c r="N63" s="102"/>
-      <c r="O63" s="102"/>
-      <c r="P63" s="102"/>
+      <c r="B63" s="104"/>
+      <c r="C63" s="104"/>
+      <c r="D63" s="104"/>
+      <c r="E63" s="104"/>
+      <c r="F63" s="104"/>
+      <c r="G63" s="104"/>
+      <c r="H63" s="104"/>
+      <c r="I63" s="104"/>
+      <c r="J63" s="104"/>
+      <c r="K63" s="104"/>
+      <c r="L63" s="104"/>
+      <c r="M63" s="104"/>
+      <c r="N63" s="104"/>
+      <c r="O63" s="104"/>
+      <c r="P63" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4828,172 +4682,32 @@
     <mergeCell ref="K5:M5"/>
     <mergeCell ref="N5:P5"/>
   </mergeCells>
-  <conditionalFormatting sqref="B11:D12 N11:P12 B34:D34 B31:B33 O34:P34 N59:P59 B59:D59 B58 B60 N19:P25 B22:D25 B10 N14:P16 B14:D16 B13 B17 B30:D30 N30:P30 B28 O36:P37 B36:D37 B35 B40:D50 O40:P50 B38:B39 B27:D27 B26 N27:P27 O52:P57 B52:D57 B51 C19:D21 G52:K57 G27:K27 G40:K50 G36:K37 G30:K30 G14:K16 G19:K25 G59:K59 G34:K34 G11:K12">
-    <cfRule type="cellIs" dxfId="33" priority="34" operator="lessThan">
+  <conditionalFormatting sqref="B28">
+    <cfRule type="cellIs" dxfId="5" priority="34" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M11:M12 M34 M59 M19:M25 M14:M16 M30 M36:M37 M40:M50 M27 M52:M57">
-    <cfRule type="cellIs" dxfId="32" priority="33" operator="lessThan">
+  <conditionalFormatting sqref="B11:D27">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L11:L12 L34 L59 L19:L25 L14:L16 L30 L36:L37 L40:L50 L27 L52:L57">
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="lessThan">
+  <conditionalFormatting sqref="B30:D60">
+    <cfRule type="cellIs" dxfId="3" priority="15" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="cellIs" dxfId="30" priority="31" operator="lessThan">
+  <conditionalFormatting sqref="B10:E10 E11:E62">
+    <cfRule type="cellIs" dxfId="2" priority="25" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31 G31:P31">
-    <cfRule type="cellIs" dxfId="29" priority="30" operator="lessThan">
+  <conditionalFormatting sqref="C28:D29">
+    <cfRule type="cellIs" dxfId="1" priority="21" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33:D33 G33:P33">
-    <cfRule type="cellIs" dxfId="28" priority="29" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58:D58 G58:P58">
-    <cfRule type="cellIs" dxfId="27" priority="28" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60:D60 G60:P60">
-    <cfRule type="cellIs" dxfId="26" priority="27" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17:D17 G17:P17">
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10:E10 G10:P10 E11:E62">
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13:D13 G13:O13">
-    <cfRule type="cellIs" dxfId="23" priority="24" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18:D18 G18:P18">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C28:D28 G28:P28">
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29:D29 G29:P29">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35:D35 O35:P35 G35:M35">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:D38 O38:P38 G38:M38">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C39:D39 O39:P39 G39:M39">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32:D32 G32:P32">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26:D26 G26:P26">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51:D51 O51:P51 G51:M51">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P13">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N35:N36 N43:N49 N38:N40 N54 N51">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N55">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N57">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N41">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N34">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N37">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N42">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N52">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N53">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N56">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N50">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18:B21">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10:F60">
+  <conditionalFormatting sqref="F10:P60">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -5010,7 +4724,9 @@
   </sheetPr>
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5054,13 +4770,16 @@
         <v>5.5878521842202787E-3</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <f>'Table MV-1'!$P10/'Table MV-1'!$P$61</f>
+        <v>1.9282655873447636E-2</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <f>'Table MV-1'!$P10/'Table MV-1'!$P$61</f>
+        <v>1.9282655873447636E-2</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <f>'Table MV-1'!$P10/'Table MV-1'!$P$61</f>
+        <v>1.9282655873447636E-2</v>
       </c>
       <c r="G2">
         <f>'Table MV-1'!M10/'Table MV-1'!$M$61</f>
@@ -5080,13 +4799,16 @@
         <v>8.5645956308639404E-3</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <f>'Table MV-1'!$P11/'Table MV-1'!$P$61</f>
+        <v>2.8734612685508815E-3</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <f>'Table MV-1'!$P11/'Table MV-1'!$P$61</f>
+        <v>2.8734612685508815E-3</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <f>'Table MV-1'!$P11/'Table MV-1'!$P$61</f>
+        <v>2.8734612685508815E-3</v>
       </c>
       <c r="G3">
         <f>'Table MV-1'!M11/'Table MV-1'!$M$61</f>
@@ -5106,13 +4828,16 @@
         <v>8.4314569052797456E-3</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <f>'Table MV-1'!$P12/'Table MV-1'!$P$61</f>
+        <v>2.194088643887716E-2</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <f>'Table MV-1'!$P12/'Table MV-1'!$P$61</f>
+        <v>2.194088643887716E-2</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <f>'Table MV-1'!$P12/'Table MV-1'!$P$61</f>
+        <v>2.194088643887716E-2</v>
       </c>
       <c r="G4">
         <f>'Table MV-1'!M12/'Table MV-1'!$M$61</f>
@@ -5132,13 +4857,16 @@
         <v>1.1966588141313841E-2</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <f>'Table MV-1'!$P13/'Table MV-1'!$P$61</f>
+        <v>1.0559004097364129E-2</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <f>'Table MV-1'!$P13/'Table MV-1'!$P$61</f>
+        <v>1.0559004097364129E-2</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <f>'Table MV-1'!$P13/'Table MV-1'!$P$61</f>
+        <v>1.0559004097364129E-2</v>
       </c>
       <c r="G5">
         <f>'Table MV-1'!M13/'Table MV-1'!$M$61</f>
@@ -5158,13 +4886,16 @@
         <v>0.10017993599405446</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <f>'Table MV-1'!$P14/'Table MV-1'!$P$61</f>
+        <v>0.1101732172422014</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <f>'Table MV-1'!$P14/'Table MV-1'!$P$61</f>
+        <v>0.1101732172422014</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <f>'Table MV-1'!$P14/'Table MV-1'!$P$61</f>
+        <v>0.1101732172422014</v>
       </c>
       <c r="G6">
         <f>'Table MV-1'!M14/'Table MV-1'!$M$61</f>
@@ -5184,13 +4915,16 @@
         <v>1.3631815783695276E-2</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <f>'Table MV-1'!$P15/'Table MV-1'!$P$61</f>
+        <v>1.9392719458399887E-2</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <f>'Table MV-1'!$P15/'Table MV-1'!$P$61</f>
+        <v>1.9392719458399887E-2</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <f>'Table MV-1'!$P15/'Table MV-1'!$P$61</f>
+        <v>1.9392719458399887E-2</v>
       </c>
       <c r="G7">
         <f>'Table MV-1'!M15/'Table MV-1'!$M$61</f>
@@ -5210,13 +4944,16 @@
         <v>1.169732997240849E-2</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <f>'Table MV-1'!$P16/'Table MV-1'!$P$61</f>
+        <v>1.0392955521738887E-2</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <f>'Table MV-1'!$P16/'Table MV-1'!$P$61</f>
+        <v>1.0392955521738887E-2</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <f>'Table MV-1'!$P16/'Table MV-1'!$P$61</f>
+        <v>1.0392955521738887E-2</v>
       </c>
       <c r="G8">
         <f>'Table MV-1'!M16/'Table MV-1'!$M$61</f>
@@ -5236,13 +4973,16 @@
         <v>3.8341965823090428E-3</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <f>'Table MV-1'!$P17/'Table MV-1'!$P$61</f>
+        <v>3.6465629954535311E-3</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <f>'Table MV-1'!$P17/'Table MV-1'!$P$61</f>
+        <v>3.6465629954535311E-3</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <f>'Table MV-1'!$P17/'Table MV-1'!$P$61</f>
+        <v>3.6465629954535311E-3</v>
       </c>
       <c r="G9">
         <f>'Table MV-1'!M17/'Table MV-1'!$M$61</f>
@@ -5262,13 +5002,16 @@
         <v>5.1000080479378894E-3</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <f>'Table MV-1'!$P18/'Table MV-1'!$P$61</f>
+        <v>1.2922069411262062E-3</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <f>'Table MV-1'!$P18/'Table MV-1'!$P$61</f>
+        <v>1.2922069411262062E-3</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <f>'Table MV-1'!$P18/'Table MV-1'!$P$61</f>
+        <v>1.2922069411262062E-3</v>
       </c>
       <c r="G10">
         <f>'Table MV-1'!M18/'Table MV-1'!$M$61</f>
@@ -5288,13 +5031,16 @@
         <v>5.9786242795356839E-2</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <f>'Table MV-1'!$P19/'Table MV-1'!$P$61</f>
+        <v>6.6921421388709962E-2</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <f>'Table MV-1'!$P19/'Table MV-1'!$P$61</f>
+        <v>6.6921421388709962E-2</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <f>'Table MV-1'!$P19/'Table MV-1'!$P$61</f>
+        <v>6.6921421388709962E-2</v>
       </c>
       <c r="G11">
         <f>'Table MV-1'!M19/'Table MV-1'!$M$61</f>
@@ -5314,13 +5060,16 @@
         <v>3.6664815309761158E-2</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <f>'Table MV-1'!$P20/'Table MV-1'!$P$61</f>
+        <v>3.2001349757641386E-2</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <f>'Table MV-1'!$P20/'Table MV-1'!$P$61</f>
+        <v>3.2001349757641386E-2</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <f>'Table MV-1'!$P20/'Table MV-1'!$P$61</f>
+        <v>3.2001349757641386E-2</v>
       </c>
       <c r="G12">
         <f>'Table MV-1'!M20/'Table MV-1'!$M$61</f>
@@ -5340,13 +5089,16 @@
         <v>2.8664568903761568E-3</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <f>'Table MV-1'!$P21/'Table MV-1'!$P$61</f>
+        <v>4.5120524608973367E-3</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <f>'Table MV-1'!$P21/'Table MV-1'!$P$61</f>
+        <v>4.5120524608973367E-3</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <f>'Table MV-1'!$P21/'Table MV-1'!$P$61</f>
+        <v>4.5120524608973367E-3</v>
       </c>
       <c r="G13">
         <f>'Table MV-1'!M21/'Table MV-1'!$M$61</f>
@@ -5366,13 +5118,16 @@
         <v>3.782530808201743E-3</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <f>'Table MV-1'!$P22/'Table MV-1'!$P$61</f>
+        <v>6.9502899565489131E-3</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <f>'Table MV-1'!$P22/'Table MV-1'!$P$61</f>
+        <v>6.9502899565489131E-3</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <f>'Table MV-1'!$P22/'Table MV-1'!$P$61</f>
+        <v>6.9502899565489131E-3</v>
       </c>
       <c r="G14">
         <f>'Table MV-1'!M22/'Table MV-1'!$M$61</f>
@@ -5392,13 +5147,16 @@
         <v>3.2598122743969261E-2</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <f>'Table MV-1'!$P23/'Table MV-1'!$P$61</f>
+        <v>3.837338547117259E-2</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <f>'Table MV-1'!$P23/'Table MV-1'!$P$61</f>
+        <v>3.837338547117259E-2</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <f>'Table MV-1'!$P23/'Table MV-1'!$P$61</f>
+        <v>3.837338547117259E-2</v>
       </c>
       <c r="G15">
         <f>'Table MV-1'!M23/'Table MV-1'!$M$61</f>
@@ -5418,13 +5176,16 @@
         <v>2.0735859723449008E-2</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <f>'Table MV-1'!$P24/'Table MV-1'!$P$61</f>
+        <v>2.2470473208938503E-2</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <f>'Table MV-1'!$P24/'Table MV-1'!$P$61</f>
+        <v>2.2470473208938503E-2</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <f>'Table MV-1'!$P24/'Table MV-1'!$P$61</f>
+        <v>2.2470473208938503E-2</v>
       </c>
       <c r="G16">
         <f>'Table MV-1'!M24/'Table MV-1'!$M$61</f>
@@ -5444,13 +5205,16 @@
         <v>9.1140412670434948E-3</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <f>'Table MV-1'!$P25/'Table MV-1'!$P$61</f>
+        <v>1.3726141018743511E-2</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <f>'Table MV-1'!$P25/'Table MV-1'!$P$61</f>
+        <v>1.3726141018743511E-2</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <f>'Table MV-1'!$P25/'Table MV-1'!$P$61</f>
+        <v>1.3726141018743511E-2</v>
       </c>
       <c r="G17">
         <f>'Table MV-1'!M25/'Table MV-1'!$M$61</f>
@@ -5470,13 +5234,16 @@
         <v>6.5585725938901249E-3</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <f>'Table MV-1'!$P26/'Table MV-1'!$P$61</f>
+        <v>9.4360931295224514E-3</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <f>'Table MV-1'!$P26/'Table MV-1'!$P$61</f>
+        <v>9.4360931295224514E-3</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <f>'Table MV-1'!$P26/'Table MV-1'!$P$61</f>
+        <v>9.4360931295224514E-3</v>
       </c>
       <c r="G18">
         <f>'Table MV-1'!M26/'Table MV-1'!$M$61</f>
@@ -5496,13 +5263,16 @@
         <v>1.0917375497904058E-2</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <f>'Table MV-1'!$P27/'Table MV-1'!$P$61</f>
+        <v>1.6163360078298817E-2</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <f>'Table MV-1'!$P27/'Table MV-1'!$P$61</f>
+        <v>1.6163360078298817E-2</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <f>'Table MV-1'!$P27/'Table MV-1'!$P$61</f>
+        <v>1.6163360078298817E-2</v>
       </c>
       <c r="G19">
         <f>'Table MV-1'!M27/'Table MV-1'!$M$61</f>
@@ -5522,13 +5292,16 @@
         <v>2.9889643893651965E-2</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <f>'Table MV-1'!$P28/'Table MV-1'!$P$61</f>
+        <v>1.3994268785299344E-2</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <f>'Table MV-1'!$P28/'Table MV-1'!$P$61</f>
+        <v>1.3994268785299344E-2</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <f>'Table MV-1'!$P28/'Table MV-1'!$P$61</f>
+        <v>1.3994268785299344E-2</v>
       </c>
       <c r="G20">
         <f>'Table MV-1'!M28/'Table MV-1'!$M$61</f>
@@ -5548,13 +5321,16 @@
         <v>4.5932860326547567E-3</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <f>'Table MV-1'!$P29/'Table MV-1'!$P$61</f>
+        <v>4.0632555805939817E-3</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <f>'Table MV-1'!$P29/'Table MV-1'!$P$61</f>
+        <v>4.0632555805939817E-3</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <f>'Table MV-1'!$P29/'Table MV-1'!$P$61</f>
+        <v>4.0632555805939817E-3</v>
       </c>
       <c r="G21">
         <f>'Table MV-1'!M29/'Table MV-1'!$M$61</f>
@@ -5574,13 +5350,16 @@
         <v>2.2395125930356523E-2</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <f>'Table MV-1'!$P30/'Table MV-1'!$P$61</f>
+        <v>1.5263410504658027E-2</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <f>'Table MV-1'!$P30/'Table MV-1'!$P$61</f>
+        <v>1.5263410504658027E-2</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <f>'Table MV-1'!$P30/'Table MV-1'!$P$61</f>
+        <v>1.5263410504658027E-2</v>
       </c>
       <c r="G22">
         <f>'Table MV-1'!M30/'Table MV-1'!$M$61</f>
@@ -5600,13 +5379,16 @@
         <v>1.3663610106222844E-2</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <f>'Table MV-1'!$P31/'Table MV-1'!$P$61</f>
+        <v>1.8254600811341285E-2</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <f>'Table MV-1'!$P31/'Table MV-1'!$P$61</f>
+        <v>1.8254600811341285E-2</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <f>'Table MV-1'!$P31/'Table MV-1'!$P$61</f>
+        <v>1.8254600811341285E-2</v>
       </c>
       <c r="G23">
         <f>'Table MV-1'!M31/'Table MV-1'!$M$61</f>
@@ -5626,13 +5408,16 @@
         <v>8.8845260012976063E-3</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <f>'Table MV-1'!$P32/'Table MV-1'!$P$61</f>
+        <v>3.0637308640614442E-2</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <f>'Table MV-1'!$P32/'Table MV-1'!$P$61</f>
+        <v>3.0637308640614442E-2</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <f>'Table MV-1'!$P32/'Table MV-1'!$P$61</f>
+        <v>3.0637308640614442E-2</v>
       </c>
       <c r="G24">
         <f>'Table MV-1'!M32/'Table MV-1'!$M$61</f>
@@ -5652,13 +5437,16 @@
         <v>1.9068644935909602E-2</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <f>'Table MV-1'!$P33/'Table MV-1'!$P$61</f>
+        <v>2.0625139489048872E-2</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <f>'Table MV-1'!$P33/'Table MV-1'!$P$61</f>
+        <v>2.0625139489048872E-2</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <f>'Table MV-1'!$P33/'Table MV-1'!$P$61</f>
+        <v>2.0625139489048872E-2</v>
       </c>
       <c r="G25">
         <f>'Table MV-1'!M33/'Table MV-1'!$M$61</f>
@@ -5678,13 +5466,16 @@
         <v>7.3385270683945557E-3</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <f>'Table MV-1'!$P34/'Table MV-1'!$P$61</f>
+        <v>7.462400218225123E-3</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <f>'Table MV-1'!$P34/'Table MV-1'!$P$61</f>
+        <v>7.462400218225123E-3</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <f>'Table MV-1'!$P34/'Table MV-1'!$P$61</f>
+        <v>7.462400218225123E-3</v>
       </c>
       <c r="G26">
         <f>'Table MV-1'!M34/'Table MV-1'!$M$61</f>
@@ -5704,13 +5495,16 @@
         <v>3.3533074540795592E-2</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <f>'Table MV-1'!$P35/'Table MV-1'!$P$61</f>
+        <v>2.024919884507027E-2</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <f>'Table MV-1'!$P35/'Table MV-1'!$P$61</f>
+        <v>2.024919884507027E-2</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <f>'Table MV-1'!$P35/'Table MV-1'!$P$61</f>
+        <v>2.024919884507027E-2</v>
       </c>
       <c r="G27">
         <f>'Table MV-1'!M35/'Table MV-1'!$M$61</f>
@@ -5730,13 +5524,16 @@
         <v>5.1616095478350553E-3</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <f>'Table MV-1'!$P36/'Table MV-1'!$P$61</f>
+        <v>7.0766920109744495E-3</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <f>'Table MV-1'!$P36/'Table MV-1'!$P$61</f>
+        <v>7.0766920109744495E-3</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <f>'Table MV-1'!$P36/'Table MV-1'!$P$61</f>
+        <v>7.0766920109744495E-3</v>
       </c>
       <c r="G28">
         <f>'Table MV-1'!M36/'Table MV-1'!$M$61</f>
@@ -5756,13 +5553,16 @@
         <v>1.7177876318098223E-2</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <f>'Table MV-1'!$P37/'Table MV-1'!$P$61</f>
+        <v>7.0143680710759082E-3</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <f>'Table MV-1'!$P37/'Table MV-1'!$P$61</f>
+        <v>7.0143680710759082E-3</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <f>'Table MV-1'!$P37/'Table MV-1'!$P$61</f>
+        <v>7.0143680710759082E-3</v>
       </c>
       <c r="G29">
         <f>'Table MV-1'!M37/'Table MV-1'!$M$61</f>
@@ -5782,13 +5582,16 @@
         <v>3.1883744059677944E-3</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <f>'Table MV-1'!$P38/'Table MV-1'!$P$61</f>
+        <v>9.2397053063459945E-3</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <f>'Table MV-1'!$P38/'Table MV-1'!$P$61</f>
+        <v>9.2397053063459945E-3</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <f>'Table MV-1'!$P38/'Table MV-1'!$P$61</f>
+        <v>9.2397053063459945E-3</v>
       </c>
       <c r="G30">
         <f>'Table MV-1'!M38/'Table MV-1'!$M$61</f>
@@ -5808,13 +5611,16 @@
         <v>3.0602035432785312E-3</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <f>'Table MV-1'!$P39/'Table MV-1'!$P$61</f>
+        <v>4.9201517649550101E-3</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <f>'Table MV-1'!$P39/'Table MV-1'!$P$61</f>
+        <v>4.9201517649550101E-3</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <f>'Table MV-1'!$P39/'Table MV-1'!$P$61</f>
+        <v>4.9201517649550101E-3</v>
       </c>
       <c r="G31">
         <f>'Table MV-1'!M39/'Table MV-1'!$M$61</f>
@@ -5834,13 +5640,16 @@
         <v>2.5791157005332504E-2</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <f>'Table MV-1'!$P40/'Table MV-1'!$P$61</f>
+        <v>2.1768607643858712E-2</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <f>'Table MV-1'!$P40/'Table MV-1'!$P$61</f>
+        <v>2.1768607643858712E-2</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <f>'Table MV-1'!$P40/'Table MV-1'!$P$61</f>
+        <v>2.1768607643858712E-2</v>
       </c>
       <c r="G32">
         <f>'Table MV-1'!M40/'Table MV-1'!$M$61</f>
@@ -5860,13 +5669,16 @@
         <v>9.7280691208571756E-3</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <f>'Table MV-1'!$P41/'Table MV-1'!$P$61</f>
+        <v>6.4627236423600801E-3</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <f>'Table MV-1'!$P41/'Table MV-1'!$P$61</f>
+        <v>6.4627236423600801E-3</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <f>'Table MV-1'!$P41/'Table MV-1'!$P$61</f>
+        <v>6.4627236423600801E-3</v>
       </c>
       <c r="G33">
         <f>'Table MV-1'!M41/'Table MV-1'!$M$61</f>
@@ -5886,13 +5698,16 @@
         <v>8.1156995396778245E-2</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <f>'Table MV-1'!$P42/'Table MV-1'!$P$61</f>
+        <v>4.1044623748877983E-2</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <f>'Table MV-1'!$P42/'Table MV-1'!$P$61</f>
+        <v>4.1044623748877983E-2</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <f>'Table MV-1'!$P42/'Table MV-1'!$P$61</f>
+        <v>4.1044623748877983E-2</v>
       </c>
       <c r="G34">
         <f>'Table MV-1'!M42/'Table MV-1'!$M$61</f>
@@ -5912,13 +5727,16 @@
         <v>3.311776120277922E-2</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <f>'Table MV-1'!$P43/'Table MV-1'!$P$61</f>
+        <v>3.167401497304749E-2</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <f>'Table MV-1'!$P43/'Table MV-1'!$P$61</f>
+        <v>3.167401497304749E-2</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <f>'Table MV-1'!$P43/'Table MV-1'!$P$61</f>
+        <v>3.167401497304749E-2</v>
       </c>
       <c r="G35">
         <f>'Table MV-1'!M43/'Table MV-1'!$M$61</f>
@@ -5938,13 +5756,16 @@
         <v>3.6394563568276817E-3</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <f>'Table MV-1'!$P44/'Table MV-1'!$P$61</f>
+        <v>3.2585714617236724E-3</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <f>'Table MV-1'!$P44/'Table MV-1'!$P$61</f>
+        <v>3.2585714617236724E-3</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <f>'Table MV-1'!$P44/'Table MV-1'!$P$61</f>
+        <v>3.2585714617236724E-3</v>
       </c>
       <c r="G36">
         <f>'Table MV-1'!M44/'Table MV-1'!$M$61</f>
@@ -5964,13 +5785,16 @@
         <v>4.1215377721519487E-2</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <f>'Table MV-1'!$P45/'Table MV-1'!$P$61</f>
+        <v>3.8390028384176433E-2</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <f>'Table MV-1'!$P45/'Table MV-1'!$P$61</f>
+        <v>3.8390028384176433E-2</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <f>'Table MV-1'!$P45/'Table MV-1'!$P$61</f>
+        <v>3.8390028384176433E-2</v>
       </c>
       <c r="G37">
         <f>'Table MV-1'!M45/'Table MV-1'!$M$61</f>
@@ -5990,13 +5814,16 @@
         <v>2.8227396969007492E-3</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <f>'Table MV-1'!$P46/'Table MV-1'!$P$61</f>
+        <v>1.3519637696831486E-2</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <f>'Table MV-1'!$P46/'Table MV-1'!$P$61</f>
+        <v>1.3519637696831486E-2</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <f>'Table MV-1'!$P46/'Table MV-1'!$P$61</f>
+        <v>1.3519637696831486E-2</v>
       </c>
       <c r="G38">
         <f>'Table MV-1'!M46/'Table MV-1'!$M$61</f>
@@ -6016,13 +5843,16 @@
         <v>1.772632838169879E-2</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <f>'Table MV-1'!$P47/'Table MV-1'!$P$61</f>
+        <v>1.4843224067571648E-2</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <f>'Table MV-1'!$P47/'Table MV-1'!$P$61</f>
+        <v>1.4843224067571648E-2</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <f>'Table MV-1'!$P47/'Table MV-1'!$P$61</f>
+        <v>1.4843224067571648E-2</v>
       </c>
       <c r="G39">
         <f>'Table MV-1'!M47/'Table MV-1'!$M$61</f>
@@ -6042,13 +5872,16 @@
         <v>5.4911775722848888E-2</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <f>'Table MV-1'!$P48/'Table MV-1'!$P$61</f>
+        <v>3.8744741340554098E-2</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <f>'Table MV-1'!$P48/'Table MV-1'!$P$61</f>
+        <v>3.8744741340554098E-2</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <f>'Table MV-1'!$P48/'Table MV-1'!$P$61</f>
+        <v>3.8744741340554098E-2</v>
       </c>
       <c r="G40">
         <f>'Table MV-1'!M48/'Table MV-1'!$M$61</f>
@@ -6068,13 +5901,16 @@
         <v>2.3031012380907907E-3</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <f>'Table MV-1'!$P49/'Table MV-1'!$P$61</f>
+        <v>3.1409330317849157E-3</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <f>'Table MV-1'!$P49/'Table MV-1'!$P$61</f>
+        <v>3.1409330317849157E-3</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <f>'Table MV-1'!$P49/'Table MV-1'!$P$61</f>
+        <v>3.1409330317849157E-3</v>
       </c>
       <c r="G41">
         <f>'Table MV-1'!M49/'Table MV-1'!$M$61</f>
@@ -6094,13 +5930,16 @@
         <v>1.6360166085592303E-2</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <f>'Table MV-1'!$P50/'Table MV-1'!$P$61</f>
+        <v>1.6531642517752781E-2</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <f>'Table MV-1'!$P50/'Table MV-1'!$P$61</f>
+        <v>1.6531642517752781E-2</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <f>'Table MV-1'!$P50/'Table MV-1'!$P$61</f>
+        <v>1.6531642517752781E-2</v>
       </c>
       <c r="G42">
         <f>'Table MV-1'!M50/'Table MV-1'!$M$61</f>
@@ -6120,13 +5959,16 @@
         <v>2.6518452133150647E-3</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <f>'Table MV-1'!$P51/'Table MV-1'!$P$61</f>
+        <v>4.6909021621169989E-3</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <f>'Table MV-1'!$P51/'Table MV-1'!$P$61</f>
+        <v>4.6909021621169989E-3</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <f>'Table MV-1'!$P51/'Table MV-1'!$P$61</f>
+        <v>4.6909021621169989E-3</v>
       </c>
       <c r="G43">
         <f>'Table MV-1'!M51/'Table MV-1'!$M$61</f>
@@ -6146,13 +5988,16 @@
         <v>2.9370005434842007E-2</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <f>'Table MV-1'!$P52/'Table MV-1'!$P$61</f>
+        <v>2.1221790819698876E-2</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <f>'Table MV-1'!$P52/'Table MV-1'!$P$61</f>
+        <v>2.1221790819698876E-2</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <f>'Table MV-1'!$P52/'Table MV-1'!$P$61</f>
+        <v>2.1221790819698876E-2</v>
       </c>
       <c r="G44">
         <f>'Table MV-1'!M52/'Table MV-1'!$M$61</f>
@@ -6172,13 +6017,16 @@
         <v>7.0475096600093989E-2</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <f>'Table MV-1'!$P53/'Table MV-1'!$P$61</f>
+        <v>8.1255579629910979E-2</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <f>'Table MV-1'!$P53/'Table MV-1'!$P$61</f>
+        <v>8.1255579629910979E-2</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <f>'Table MV-1'!$P53/'Table MV-1'!$P$61</f>
+        <v>8.1255579629910979E-2</v>
       </c>
       <c r="G45">
         <f>'Table MV-1'!M53/'Table MV-1'!$M$61</f>
@@ -6198,13 +6046,16 @@
         <v>6.3797295296725487E-3</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <f>'Table MV-1'!$P54/'Table MV-1'!$P$61</f>
+        <v>8.9868975731671758E-3</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <f>'Table MV-1'!$P54/'Table MV-1'!$P$61</f>
+        <v>8.9868975731671758E-3</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <f>'Table MV-1'!$P54/'Table MV-1'!$P$61</f>
+        <v>8.9868975731671758E-3</v>
       </c>
       <c r="G46">
         <f>'Table MV-1'!M54/'Table MV-1'!$M$61</f>
@@ -6224,13 +6075,16 @@
         <v>1.0720648127264725E-3</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <f>'Table MV-1'!$P55/'Table MV-1'!$P$61</f>
+        <v>2.2031925927497274E-3</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <f>'Table MV-1'!$P55/'Table MV-1'!$P$61</f>
+        <v>2.2031925927497274E-3</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <f>'Table MV-1'!$P55/'Table MV-1'!$P$61</f>
+        <v>2.2031925927497274E-3</v>
       </c>
       <c r="G47">
         <f>'Table MV-1'!M55/'Table MV-1'!$M$61</f>
@@ -6250,13 +6104,16 @@
         <v>3.5235064368599529E-2</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <f>'Table MV-1'!$P56/'Table MV-1'!$P$61</f>
+        <v>2.7568275022629669E-2</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <f>'Table MV-1'!$P56/'Table MV-1'!$P$61</f>
+        <v>2.7568275022629669E-2</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <f>'Table MV-1'!$P56/'Table MV-1'!$P$61</f>
+        <v>2.7568275022629669E-2</v>
       </c>
       <c r="G48">
         <f>'Table MV-1'!M56/'Table MV-1'!$M$61</f>
@@ -6276,13 +6133,16 @@
         <v>2.4016636379262549E-2</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <f>'Table MV-1'!$P57/'Table MV-1'!$P$61</f>
+        <v>2.6303199799000584E-2</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <f>'Table MV-1'!$P57/'Table MV-1'!$P$61</f>
+        <v>2.6303199799000584E-2</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <f>'Table MV-1'!$P57/'Table MV-1'!$P$61</f>
+        <v>2.6303199799000584E-2</v>
       </c>
       <c r="G49">
         <f>'Table MV-1'!M57/'Table MV-1'!$M$61</f>
@@ -6302,13 +6162,16 @@
         <v>3.1347214867025212E-3</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <f>'Table MV-1'!$P58/'Table MV-1'!$P$61</f>
+        <v>6.0068230796770363E-3</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <f>'Table MV-1'!$P58/'Table MV-1'!$P$61</f>
+        <v>6.0068230796770363E-3</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <f>'Table MV-1'!$P58/'Table MV-1'!$P$61</f>
+        <v>6.0068230796770363E-3</v>
       </c>
       <c r="G50">
         <f>'Table MV-1'!M58/'Table MV-1'!$M$61</f>
@@ -6328,13 +6191,16 @@
         <v>1.4844967902637837E-2</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <f>'Table MV-1'!$P59/'Table MV-1'!$P$61</f>
+        <v>2.035520680727616E-2</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <f>'Table MV-1'!$P59/'Table MV-1'!$P$61</f>
+        <v>2.035520680727616E-2</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <f>'Table MV-1'!$P59/'Table MV-1'!$P$61</f>
+        <v>2.035520680727616E-2</v>
       </c>
       <c r="G51">
         <f>'Table MV-1'!M59/'Table MV-1'!$M$61</f>
@@ -6354,13 +6220,16 @@
         <v>4.0746411464237849E-3</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <f>'Table MV-1'!$P60/'Table MV-1'!$P$61</f>
+        <v>3.1206476693976084E-3</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <f>'Table MV-1'!$P60/'Table MV-1'!$P$61</f>
+        <v>3.1206476693976084E-3</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <f>'Table MV-1'!$P60/'Table MV-1'!$P$61</f>
+        <v>3.1206476693976084E-3</v>
       </c>
       <c r="G52">
         <f>'Table MV-1'!M60/'Table MV-1'!$M$61</f>
@@ -6587,7 +6456,9 @@
   </sheetPr>
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:F52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -6631,13 +6502,16 @@
         <v>1.9600927701391289E-2</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <f>'Table MV-1'!$P10/'Table MV-1'!$P$61</f>
+        <v>1.9282655873447636E-2</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <f>'Table MV-1'!$P10/'Table MV-1'!$P$61</f>
+        <v>1.9282655873447636E-2</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <f>'Table MV-1'!$P10/'Table MV-1'!$P$61</f>
+        <v>1.9282655873447636E-2</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -6656,13 +6530,16 @@
         <v>3.6314972397001131E-3</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <f>'Table MV-1'!$P11/'Table MV-1'!$P$61</f>
+        <v>2.8734612685508815E-3</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <f>'Table MV-1'!$P11/'Table MV-1'!$P$61</f>
+        <v>2.8734612685508815E-3</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <f>'Table MV-1'!$P11/'Table MV-1'!$P$61</f>
+        <v>2.8734612685508815E-3</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -6681,13 +6558,16 @@
         <v>2.1767409304149131E-2</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <f>'Table MV-1'!$P12/'Table MV-1'!$P$61</f>
+        <v>2.194088643887716E-2</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <f>'Table MV-1'!$P12/'Table MV-1'!$P$61</f>
+        <v>2.194088643887716E-2</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <f>'Table MV-1'!$P12/'Table MV-1'!$P$61</f>
+        <v>2.194088643887716E-2</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -6706,13 +6586,16 @@
         <v>1.1515440266444459E-2</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <f>'Table MV-1'!$P13/'Table MV-1'!$P$61</f>
+        <v>1.0559004097364129E-2</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <f>'Table MV-1'!$P13/'Table MV-1'!$P$61</f>
+        <v>1.0559004097364129E-2</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <f>'Table MV-1'!$P13/'Table MV-1'!$P$61</f>
+        <v>1.0559004097364129E-2</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -6731,13 +6614,16 @@
         <v>9.483573703336938E-2</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <f>'Table MV-1'!$P14/'Table MV-1'!$P$61</f>
+        <v>0.1101732172422014</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <f>'Table MV-1'!$P14/'Table MV-1'!$P$61</f>
+        <v>0.1101732172422014</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <f>'Table MV-1'!$P14/'Table MV-1'!$P$61</f>
+        <v>0.1101732172422014</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -6756,13 +6642,16 @@
         <v>2.17963420575671E-2</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <f>'Table MV-1'!$P15/'Table MV-1'!$P$61</f>
+        <v>1.9392719458399887E-2</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <f>'Table MV-1'!$P15/'Table MV-1'!$P$61</f>
+        <v>1.9392719458399887E-2</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <f>'Table MV-1'!$P15/'Table MV-1'!$P$61</f>
+        <v>1.9392719458399887E-2</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -6781,13 +6670,16 @@
         <v>9.6855101995915252E-3</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <f>'Table MV-1'!$P16/'Table MV-1'!$P$61</f>
+        <v>1.0392955521738887E-2</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <f>'Table MV-1'!$P16/'Table MV-1'!$P$61</f>
+        <v>1.0392955521738887E-2</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <f>'Table MV-1'!$P16/'Table MV-1'!$P$61</f>
+        <v>1.0392955521738887E-2</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -6806,13 +6698,16 @@
         <v>3.607073808587494E-3</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <f>'Table MV-1'!$P17/'Table MV-1'!$P$61</f>
+        <v>3.6465629954535311E-3</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <f>'Table MV-1'!$P17/'Table MV-1'!$P$61</f>
+        <v>3.6465629954535311E-3</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <f>'Table MV-1'!$P17/'Table MV-1'!$P$61</f>
+        <v>3.6465629954535311E-3</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -6831,13 +6726,16 @@
         <v>8.5193982126037439E-4</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <f>'Table MV-1'!$P18/'Table MV-1'!$P$61</f>
+        <v>1.2922069411262062E-3</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <f>'Table MV-1'!$P18/'Table MV-1'!$P$61</f>
+        <v>1.2922069411262062E-3</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <f>'Table MV-1'!$P18/'Table MV-1'!$P$61</f>
+        <v>1.2922069411262062E-3</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -6856,13 +6754,16 @@
         <v>6.1586335732623156E-2</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <f>'Table MV-1'!$P19/'Table MV-1'!$P$61</f>
+        <v>6.6921421388709962E-2</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <f>'Table MV-1'!$P19/'Table MV-1'!$P$61</f>
+        <v>6.6921421388709962E-2</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <f>'Table MV-1'!$P19/'Table MV-1'!$P$61</f>
+        <v>6.6921421388709962E-2</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -6881,13 +6782,16 @@
         <v>3.1525712849526988E-2</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <f>'Table MV-1'!$P20/'Table MV-1'!$P$61</f>
+        <v>3.2001349757641386E-2</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <f>'Table MV-1'!$P20/'Table MV-1'!$P$61</f>
+        <v>3.2001349757641386E-2</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <f>'Table MV-1'!$P20/'Table MV-1'!$P$61</f>
+        <v>3.2001349757641386E-2</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -6906,13 +6810,16 @@
         <v>4.5222742187277015E-3</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <f>'Table MV-1'!$P21/'Table MV-1'!$P$61</f>
+        <v>4.5120524608973367E-3</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <f>'Table MV-1'!$P21/'Table MV-1'!$P$61</f>
+        <v>4.5120524608973367E-3</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <f>'Table MV-1'!$P21/'Table MV-1'!$P$61</f>
+        <v>4.5120524608973367E-3</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -6931,13 +6838,16 @@
         <v>7.8435139790973586E-3</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <f>'Table MV-1'!$P22/'Table MV-1'!$P$61</f>
+        <v>6.9502899565489131E-3</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <f>'Table MV-1'!$P22/'Table MV-1'!$P$61</f>
+        <v>6.9502899565489131E-3</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <f>'Table MV-1'!$P22/'Table MV-1'!$P$61</f>
+        <v>6.9502899565489131E-3</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -6956,13 +6866,16 @@
         <v>3.7864302450454933E-2</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <f>'Table MV-1'!$P23/'Table MV-1'!$P$61</f>
+        <v>3.837338547117259E-2</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <f>'Table MV-1'!$P23/'Table MV-1'!$P$61</f>
+        <v>3.837338547117259E-2</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <f>'Table MV-1'!$P23/'Table MV-1'!$P$61</f>
+        <v>3.837338547117259E-2</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -6981,13 +6894,16 @@
         <v>2.3819250059067168E-2</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <f>'Table MV-1'!$P24/'Table MV-1'!$P$61</f>
+        <v>2.2470473208938503E-2</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <f>'Table MV-1'!$P24/'Table MV-1'!$P$61</f>
+        <v>2.2470473208938503E-2</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <f>'Table MV-1'!$P24/'Table MV-1'!$P$61</f>
+        <v>2.2470473208938503E-2</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -7006,13 +6922,16 @@
         <v>1.5005240724472678E-2</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <f>'Table MV-1'!$P25/'Table MV-1'!$P$61</f>
+        <v>1.3726141018743511E-2</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <f>'Table MV-1'!$P25/'Table MV-1'!$P$61</f>
+        <v>1.3726141018743511E-2</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <f>'Table MV-1'!$P25/'Table MV-1'!$P$61</f>
+        <v>1.3726141018743511E-2</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -7031,13 +6950,16 @@
         <v>1.0017236512864749E-2</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <f>'Table MV-1'!$P26/'Table MV-1'!$P$61</f>
+        <v>9.4360931295224514E-3</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <f>'Table MV-1'!$P26/'Table MV-1'!$P$61</f>
+        <v>9.4360931295224514E-3</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <f>'Table MV-1'!$P26/'Table MV-1'!$P$61</f>
+        <v>9.4360931295224514E-3</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -7056,13 +6978,16 @@
         <v>1.6767766333459132E-2</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <f>'Table MV-1'!$P27/'Table MV-1'!$P$61</f>
+        <v>1.6163360078298817E-2</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <f>'Table MV-1'!$P27/'Table MV-1'!$P$61</f>
+        <v>1.6163360078298817E-2</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <f>'Table MV-1'!$P27/'Table MV-1'!$P$61</f>
+        <v>1.6163360078298817E-2</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -7081,13 +7006,16 @@
         <v>1.4952243799136747E-2</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <f>'Table MV-1'!$P28/'Table MV-1'!$P$61</f>
+        <v>1.3994268785299344E-2</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <f>'Table MV-1'!$P28/'Table MV-1'!$P$61</f>
+        <v>1.3994268785299344E-2</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <f>'Table MV-1'!$P28/'Table MV-1'!$P$61</f>
+        <v>1.3994268785299344E-2</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -7106,13 +7034,16 @@
         <v>4.472553985012004E-3</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <f>'Table MV-1'!$P29/'Table MV-1'!$P$61</f>
+        <v>4.0632555805939817E-3</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <f>'Table MV-1'!$P29/'Table MV-1'!$P$61</f>
+        <v>4.0632555805939817E-3</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <f>'Table MV-1'!$P29/'Table MV-1'!$P$61</f>
+        <v>4.0632555805939817E-3</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -7131,13 +7062,16 @@
         <v>1.3953713838208291E-2</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <f>'Table MV-1'!$P30/'Table MV-1'!$P$61</f>
+        <v>1.5263410504658027E-2</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <f>'Table MV-1'!$P30/'Table MV-1'!$P$61</f>
+        <v>1.5263410504658027E-2</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <f>'Table MV-1'!$P30/'Table MV-1'!$P$61</f>
+        <v>1.5263410504658027E-2</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -7156,13 +7090,16 @@
         <v>1.7847984402303698E-2</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <f>'Table MV-1'!$P31/'Table MV-1'!$P$61</f>
+        <v>1.8254600811341285E-2</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <f>'Table MV-1'!$P31/'Table MV-1'!$P$61</f>
+        <v>1.8254600811341285E-2</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <f>'Table MV-1'!$P31/'Table MV-1'!$P$61</f>
+        <v>1.8254600811341285E-2</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -7181,13 +7118,16 @@
         <v>3.4161287854521931E-2</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <f>'Table MV-1'!$P32/'Table MV-1'!$P$61</f>
+        <v>3.0637308640614442E-2</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <f>'Table MV-1'!$P32/'Table MV-1'!$P$61</f>
+        <v>3.0637308640614442E-2</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <f>'Table MV-1'!$P32/'Table MV-1'!$P$61</f>
+        <v>3.0637308640614442E-2</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -7206,13 +7146,16 @@
         <v>2.221147844524117E-2</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <f>'Table MV-1'!$P33/'Table MV-1'!$P$61</f>
+        <v>2.0625139489048872E-2</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <f>'Table MV-1'!$P33/'Table MV-1'!$P$61</f>
+        <v>2.0625139489048872E-2</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <f>'Table MV-1'!$P33/'Table MV-1'!$P$61</f>
+        <v>2.0625139489048872E-2</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -7231,13 +7174,16 @@
         <v>7.63482155174601E-3</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <f>'Table MV-1'!$P34/'Table MV-1'!$P$61</f>
+        <v>7.462400218225123E-3</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <f>'Table MV-1'!$P34/'Table MV-1'!$P$61</f>
+        <v>7.462400218225123E-3</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <f>'Table MV-1'!$P34/'Table MV-1'!$P$61</f>
+        <v>7.462400218225123E-3</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -7256,13 +7202,16 @@
         <v>2.1277992980917738E-2</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <f>'Table MV-1'!$P35/'Table MV-1'!$P$61</f>
+        <v>2.024919884507027E-2</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <f>'Table MV-1'!$P35/'Table MV-1'!$P$61</f>
+        <v>2.024919884507027E-2</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <f>'Table MV-1'!$P35/'Table MV-1'!$P$61</f>
+        <v>2.024919884507027E-2</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -7281,13 +7230,16 @@
         <v>7.0185743445526595E-3</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <f>'Table MV-1'!$P36/'Table MV-1'!$P$61</f>
+        <v>7.0766920109744495E-3</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <f>'Table MV-1'!$P36/'Table MV-1'!$P$61</f>
+        <v>7.0766920109744495E-3</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <f>'Table MV-1'!$P36/'Table MV-1'!$P$61</f>
+        <v>7.0766920109744495E-3</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -7306,13 +7258,16 @@
         <v>7.6979830346411097E-3</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <f>'Table MV-1'!$P37/'Table MV-1'!$P$61</f>
+        <v>7.0143680710759082E-3</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <f>'Table MV-1'!$P37/'Table MV-1'!$P$61</f>
+        <v>7.0143680710759082E-3</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <f>'Table MV-1'!$P37/'Table MV-1'!$P$61</f>
+        <v>7.0143680710759082E-3</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -7331,13 +7286,16 @@
         <v>8.9770758442244206E-3</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <f>'Table MV-1'!$P38/'Table MV-1'!$P$61</f>
+        <v>9.2397053063459945E-3</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <f>'Table MV-1'!$P38/'Table MV-1'!$P$61</f>
+        <v>9.2397053063459945E-3</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <f>'Table MV-1'!$P38/'Table MV-1'!$P$61</f>
+        <v>9.2397053063459945E-3</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -7356,13 +7314,16 @@
         <v>5.0478518381385203E-3</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <f>'Table MV-1'!$P39/'Table MV-1'!$P$61</f>
+        <v>4.9201517649550101E-3</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <f>'Table MV-1'!$P39/'Table MV-1'!$P$61</f>
+        <v>4.9201517649550101E-3</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <f>'Table MV-1'!$P39/'Table MV-1'!$P$61</f>
+        <v>4.9201517649550101E-3</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -7381,13 +7342,16 @@
         <v>2.0550771847319699E-2</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <f>'Table MV-1'!$P40/'Table MV-1'!$P$61</f>
+        <v>2.1768607643858712E-2</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <f>'Table MV-1'!$P40/'Table MV-1'!$P$61</f>
+        <v>2.1768607643858712E-2</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <f>'Table MV-1'!$P40/'Table MV-1'!$P$61</f>
+        <v>2.1768607643858712E-2</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -7406,13 +7370,16 @@
         <v>6.7792148090505171E-3</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <f>'Table MV-1'!$P41/'Table MV-1'!$P$61</f>
+        <v>6.4627236423600801E-3</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <f>'Table MV-1'!$P41/'Table MV-1'!$P$61</f>
+        <v>6.4627236423600801E-3</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <f>'Table MV-1'!$P41/'Table MV-1'!$P$61</f>
+        <v>6.4627236423600801E-3</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -7431,13 +7398,16 @@
         <v>4.1040438660927506E-2</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <f>'Table MV-1'!$P42/'Table MV-1'!$P$61</f>
+        <v>4.1044623748877983E-2</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <f>'Table MV-1'!$P42/'Table MV-1'!$P$61</f>
+        <v>4.1044623748877983E-2</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <f>'Table MV-1'!$P42/'Table MV-1'!$P$61</f>
+        <v>4.1044623748877983E-2</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -7456,13 +7426,16 @@
         <v>3.1700275653385936E-2</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <f>'Table MV-1'!$P43/'Table MV-1'!$P$61</f>
+        <v>3.167401497304749E-2</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <f>'Table MV-1'!$P43/'Table MV-1'!$P$61</f>
+        <v>3.167401497304749E-2</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <f>'Table MV-1'!$P43/'Table MV-1'!$P$61</f>
+        <v>3.167401497304749E-2</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -7481,13 +7454,16 @@
         <v>3.986117035446643E-3</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <f>'Table MV-1'!$P44/'Table MV-1'!$P$61</f>
+        <v>3.2585714617236724E-3</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <f>'Table MV-1'!$P44/'Table MV-1'!$P$61</f>
+        <v>3.2585714617236724E-3</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <f>'Table MV-1'!$P44/'Table MV-1'!$P$61</f>
+        <v>3.2585714617236724E-3</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -7506,13 +7482,16 @@
         <v>3.6683925395789657E-2</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <f>'Table MV-1'!$P45/'Table MV-1'!$P$61</f>
+        <v>3.8390028384176433E-2</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <f>'Table MV-1'!$P45/'Table MV-1'!$P$61</f>
+        <v>3.8390028384176433E-2</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <f>'Table MV-1'!$P45/'Table MV-1'!$P$61</f>
+        <v>3.8390028384176433E-2</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -7531,13 +7510,16 @@
         <v>1.4677986568760525E-2</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <f>'Table MV-1'!$P46/'Table MV-1'!$P$61</f>
+        <v>1.3519637696831486E-2</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <f>'Table MV-1'!$P46/'Table MV-1'!$P$61</f>
+        <v>1.3519637696831486E-2</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <f>'Table MV-1'!$P46/'Table MV-1'!$P$61</f>
+        <v>1.3519637696831486E-2</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -7556,13 +7538,16 @@
         <v>1.5566676127984676E-2</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <f>'Table MV-1'!$P47/'Table MV-1'!$P$61</f>
+        <v>1.4843224067571648E-2</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <f>'Table MV-1'!$P47/'Table MV-1'!$P$61</f>
+        <v>1.4843224067571648E-2</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <f>'Table MV-1'!$P47/'Table MV-1'!$P$61</f>
+        <v>1.4843224067571648E-2</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -7581,13 +7566,16 @@
         <v>3.8593803021701831E-2</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <f>'Table MV-1'!$P48/'Table MV-1'!$P$61</f>
+        <v>3.8744741340554098E-2</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <f>'Table MV-1'!$P48/'Table MV-1'!$P$61</f>
+        <v>3.8744741340554098E-2</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <f>'Table MV-1'!$P48/'Table MV-1'!$P$61</f>
+        <v>3.8744741340554098E-2</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -7606,13 +7594,16 @@
         <v>2.8426879307146095E-3</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <f>'Table MV-1'!$P49/'Table MV-1'!$P$61</f>
+        <v>3.1409330317849157E-3</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <f>'Table MV-1'!$P49/'Table MV-1'!$P$61</f>
+        <v>3.1409330317849157E-3</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <f>'Table MV-1'!$P49/'Table MV-1'!$P$61</f>
+        <v>3.1409330317849157E-3</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -7631,13 +7622,16 @@
         <v>1.6494772704388254E-2</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <f>'Table MV-1'!$P50/'Table MV-1'!$P$61</f>
+        <v>1.6531642517752781E-2</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <f>'Table MV-1'!$P50/'Table MV-1'!$P$61</f>
+        <v>1.6531642517752781E-2</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <f>'Table MV-1'!$P50/'Table MV-1'!$P$61</f>
+        <v>1.6531642517752781E-2</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -7656,13 +7650,16 @@
         <v>5.1835093488657516E-3</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <f>'Table MV-1'!$P51/'Table MV-1'!$P$61</f>
+        <v>4.6909021621169989E-3</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <f>'Table MV-1'!$P51/'Table MV-1'!$P$61</f>
+        <v>4.6909021621169989E-3</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <f>'Table MV-1'!$P51/'Table MV-1'!$P$61</f>
+        <v>4.6909021621169989E-3</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -7681,13 +7678,16 @@
         <v>2.1883288976798098E-2</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <f>'Table MV-1'!$P52/'Table MV-1'!$P$61</f>
+        <v>2.1221790819698876E-2</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <f>'Table MV-1'!$P52/'Table MV-1'!$P$61</f>
+        <v>2.1221790819698876E-2</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <f>'Table MV-1'!$P52/'Table MV-1'!$P$61</f>
+        <v>2.1221790819698876E-2</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -7706,13 +7706,16 @@
         <v>8.6297781225124395E-2</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <f>'Table MV-1'!$P53/'Table MV-1'!$P$61</f>
+        <v>8.1255579629910979E-2</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <f>'Table MV-1'!$P53/'Table MV-1'!$P$61</f>
+        <v>8.1255579629910979E-2</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <f>'Table MV-1'!$P53/'Table MV-1'!$P$61</f>
+        <v>8.1255579629910979E-2</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -7731,13 +7734,16 @@
         <v>8.9600234207263124E-3</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <f>'Table MV-1'!$P54/'Table MV-1'!$P$61</f>
+        <v>8.9868975731671758E-3</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <f>'Table MV-1'!$P54/'Table MV-1'!$P$61</f>
+        <v>8.9868975731671758E-3</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <f>'Table MV-1'!$P54/'Table MV-1'!$P$61</f>
+        <v>8.9868975731671758E-3</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -7756,13 +7762,16 @@
         <v>2.3814053188992734E-3</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <f>'Table MV-1'!$P55/'Table MV-1'!$P$61</f>
+        <v>2.2031925927497274E-3</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <f>'Table MV-1'!$P55/'Table MV-1'!$P$61</f>
+        <v>2.2031925927497274E-3</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <f>'Table MV-1'!$P55/'Table MV-1'!$P$61</f>
+        <v>2.2031925927497274E-3</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -7781,13 +7790,16 @@
         <v>2.6816184066770478E-2</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <f>'Table MV-1'!$P56/'Table MV-1'!$P$61</f>
+        <v>2.7568275022629669E-2</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <f>'Table MV-1'!$P56/'Table MV-1'!$P$61</f>
+        <v>2.7568275022629669E-2</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <f>'Table MV-1'!$P56/'Table MV-1'!$P$61</f>
+        <v>2.7568275022629669E-2</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -7806,13 +7818,16 @@
         <v>2.6086002141878541E-2</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <f>'Table MV-1'!$P57/'Table MV-1'!$P$61</f>
+        <v>2.6303199799000584E-2</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <f>'Table MV-1'!$P57/'Table MV-1'!$P$61</f>
+        <v>2.6303199799000584E-2</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <f>'Table MV-1'!$P57/'Table MV-1'!$P$61</f>
+        <v>2.6303199799000584E-2</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -7831,13 +7846,16 @@
         <v>6.8260176103406393E-3</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <f>'Table MV-1'!$P58/'Table MV-1'!$P$61</f>
+        <v>6.0068230796770363E-3</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <f>'Table MV-1'!$P58/'Table MV-1'!$P$61</f>
+        <v>6.0068230796770363E-3</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <f>'Table MV-1'!$P58/'Table MV-1'!$P$61</f>
+        <v>6.0068230796770363E-3</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -7856,13 +7874,16 @@
         <v>2.1205726135675299E-2</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <f>'Table MV-1'!$P59/'Table MV-1'!$P$61</f>
+        <v>2.035520680727616E-2</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <f>'Table MV-1'!$P59/'Table MV-1'!$P$61</f>
+        <v>2.035520680727616E-2</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <f>'Table MV-1'!$P59/'Table MV-1'!$P$61</f>
+        <v>2.035520680727616E-2</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -7881,13 +7902,16 @@
         <v>3.9463197884523288E-3</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <f>'Table MV-1'!$P60/'Table MV-1'!$P$61</f>
+        <v>3.1206476693976084E-3</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <f>'Table MV-1'!$P60/'Table MV-1'!$P$61</f>
+        <v>3.1206476693976084E-3</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <f>'Table MV-1'!$P60/'Table MV-1'!$P$61</f>
+        <v>3.1206476693976084E-3</v>
       </c>
       <c r="G52">
         <v>0</v>

</xml_diff>

<commit_message>
Subscripts differential financing lever by industry category (#352)
</commit_message>
<xml_diff>
--- a/InputData/trans/VSbS/Vehicle Shares by Subregion.xlsx
+++ b/InputData/trans/VSbS/Vehicle Shares by Subregion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\VSbS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\trans\VSbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E91793-1818-4D44-889A-A4ABF3FC1BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AA5D4D-74B3-4477-98B8-51707E087857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F34BB550-7D2B-439D-9C81-D72ED5B29ABD}"/>
+    <workbookView xWindow="34005" yWindow="1710" windowWidth="23010" windowHeight="14205" activeTab="1" xr2:uid="{F34BB550-7D2B-439D-9C81-D72ED5B29ABD}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -286,9 +286,6 @@
     <t>June 2022</t>
   </si>
   <si>
-    <t>STATE MOTOR-VEHICLE REGISTRATIONS - 2020</t>
-  </si>
-  <si>
     <t>LDVs</t>
   </si>
   <si>
@@ -380,15 +377,19 @@
   </si>
   <si>
     <t>U.S. Data Notes</t>
+  </si>
+  <si>
+    <t>2022 State Motor-Vehicle Registrations (1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0_);[Red]\(#,##0\);\—_)"/>
+    <numFmt numFmtId="168" formatCode="#,##0.000_);\(#,##0.000\)"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -1013,26 +1014,6 @@
       <right style="thin">
         <color theme="1"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
@@ -1065,6 +1046,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1075,7 +1082,7 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="37" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -1249,31 +1256,32 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="37" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="8" fillId="0" borderId="48" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="8" fillId="0" borderId="47" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="37" fontId="8" fillId="0" borderId="46" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="37" fontId="5" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="8" fillId="0" borderId="45" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="8" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="5" fillId="0" borderId="47" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="37" fontId="5" fillId="0" borderId="45" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="37" fontId="5" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="5" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="37" fontId="5" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="5" fillId="0" borderId="48" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="37" fontId="5" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="5" fillId="0" borderId="46" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1286,7 +1294,37 @@
     <cellStyle name="Normal 5" xfId="6" xr:uid="{58A5829F-0798-4AC5-A887-3CBCA8BB0153}"/>
     <cellStyle name="Normal 8 2" xfId="4" xr:uid="{1E08BF75-563B-4006-9FB0-94126509CFF1}"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1331,9 +1369,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1371,7 +1409,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1477,7 +1515,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1619,7 +1657,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1629,11 +1667,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B0F8C0-DE1A-4000-9351-A11EE8CD5BC4}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="70.140625" customWidth="1"/>
+    <col min="2" max="2" width="70.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1671,22 +1711,22 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="102" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13" s="103"/>
     </row>
@@ -1695,48 +1735,48 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="100" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B23" s="101"/>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1750,40 +1790,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949F6402-DD66-4CAC-8910-748EA4AEB83B}">
-  <dimension ref="A1:P63"/>
+  <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:P1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="8.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="8"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="4" customWidth="1"/>
-    <col min="2" max="16" width="9.85546875" style="4" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="11.26953125" style="4" customWidth="1"/>
+    <col min="2" max="16" width="9.81640625" style="4" customWidth="1"/>
+    <col min="17" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15">
-      <c r="A1" s="105" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-    </row>
-    <row r="2" spans="1:16">
+    <row r="1" spans="1:17" ht="14">
+      <c r="A1" s="114" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="114"/>
+      <c r="P1" s="114"/>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="98"/>
       <c r="B2" s="96"/>
       <c r="C2" s="96"/>
@@ -1801,7 +1841,7 @@
       <c r="O2" s="96"/>
       <c r="P2" s="96"/>
     </row>
-    <row r="3" spans="1:16" ht="9">
+    <row r="3" spans="1:17" ht="9">
       <c r="A3" s="97" t="s">
         <v>75</v>
       </c>
@@ -1823,55 +1863,55 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17">
       <c r="A4" s="94"/>
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="107"/>
-      <c r="D4" s="107"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="107"/>
-      <c r="I4" s="107"/>
-      <c r="J4" s="107"/>
-      <c r="K4" s="107"/>
-      <c r="L4" s="107"/>
-      <c r="M4" s="107"/>
-      <c r="N4" s="107"/>
-      <c r="O4" s="107"/>
-      <c r="P4" s="108"/>
-    </row>
-    <row r="5" spans="1:16" ht="9">
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="106"/>
+      <c r="M4" s="106"/>
+      <c r="N4" s="106"/>
+      <c r="O4" s="106"/>
+      <c r="P4" s="107"/>
+    </row>
+    <row r="5" spans="1:17" ht="9">
       <c r="A5" s="79"/>
-      <c r="B5" s="109" t="s">
+      <c r="B5" s="112" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="110"/>
-      <c r="D5" s="110"/>
-      <c r="E5" s="111" t="s">
+      <c r="C5" s="109"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="108" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="110"/>
-      <c r="G5" s="112"/>
-      <c r="H5" s="110" t="s">
+      <c r="F5" s="109"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="108" t="s">
         <v>71</v>
       </c>
-      <c r="I5" s="110"/>
-      <c r="J5" s="110"/>
-      <c r="K5" s="111" t="s">
+      <c r="I5" s="109"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="108" t="s">
         <v>70</v>
       </c>
-      <c r="L5" s="110"/>
-      <c r="M5" s="112"/>
-      <c r="N5" s="110" t="s">
+      <c r="L5" s="109"/>
+      <c r="M5" s="111"/>
+      <c r="N5" s="108" t="s">
         <v>69</v>
       </c>
-      <c r="O5" s="110"/>
-      <c r="P5" s="113"/>
-    </row>
-    <row r="6" spans="1:16" ht="9">
+      <c r="O5" s="109"/>
+      <c r="P5" s="110"/>
+    </row>
+    <row r="6" spans="1:17" ht="9">
       <c r="A6" s="79" t="s">
         <v>68</v>
       </c>
@@ -1899,7 +1939,7 @@
       <c r="O6" s="88"/>
       <c r="P6" s="87"/>
     </row>
-    <row r="7" spans="1:16" ht="9">
+    <row r="7" spans="1:17" ht="9">
       <c r="A7" s="79"/>
       <c r="B7" s="79" t="s">
         <v>63</v>
@@ -1945,7 +1985,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="9">
+    <row r="8" spans="1:17" ht="9">
       <c r="A8" s="79"/>
       <c r="B8" s="79" t="s">
         <v>65</v>
@@ -1992,8 +2032,9 @@
       <c r="P8" s="81" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="9">
+      <c r="Q8" s="113"/>
+    </row>
+    <row r="9" spans="1:17" ht="9">
       <c r="A9" s="74"/>
       <c r="B9" s="74" t="s">
         <v>60</v>
@@ -2033,7 +2074,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="9">
+    <row r="10" spans="1:17" ht="9">
       <c r="A10" s="19" t="s">
         <v>58</v>
       </c>
@@ -2082,8 +2123,9 @@
       <c r="P10" s="12">
         <v>5320340</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" ht="9">
+      <c r="Q10" s="113"/>
+    </row>
+    <row r="11" spans="1:17" ht="9">
       <c r="A11" s="19" t="s">
         <v>57</v>
       </c>
@@ -2132,8 +2174,9 @@
       <c r="P11" s="20">
         <v>792826</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="9">
+      <c r="Q11" s="113"/>
+    </row>
+    <row r="12" spans="1:17" ht="9">
       <c r="A12" s="19" t="s">
         <v>56</v>
       </c>
@@ -2182,8 +2225,9 @@
       <c r="P12" s="20">
         <v>6053781</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="9">
+      <c r="Q12" s="113"/>
+    </row>
+    <row r="13" spans="1:17" ht="9">
       <c r="A13" s="19" t="s">
         <v>55</v>
       </c>
@@ -2232,8 +2276,9 @@
       <c r="P13" s="31">
         <v>2913369</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="9">
+      <c r="Q13" s="113"/>
+    </row>
+    <row r="14" spans="1:17" ht="9">
       <c r="A14" s="52" t="s">
         <v>54</v>
       </c>
@@ -2282,8 +2327,9 @@
       <c r="P14" s="20">
         <v>30398249</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="9">
+      <c r="Q14" s="113"/>
+    </row>
+    <row r="15" spans="1:17" ht="9">
       <c r="A15" s="19" t="s">
         <v>53</v>
       </c>
@@ -2332,8 +2378,9 @@
       <c r="P15" s="20">
         <v>5350708</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" ht="9">
+      <c r="Q15" s="113"/>
+    </row>
+    <row r="16" spans="1:17" ht="9">
       <c r="A16" s="19" t="s">
         <v>52</v>
       </c>
@@ -2382,8 +2429,9 @@
       <c r="P16" s="20">
         <v>2867554</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" ht="9">
+      <c r="Q16" s="113"/>
+    </row>
+    <row r="17" spans="1:17" ht="9">
       <c r="A17" s="43" t="s">
         <v>51</v>
       </c>
@@ -2432,8 +2480,9 @@
       <c r="P17" s="42">
         <v>1006135</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" ht="9">
+      <c r="Q17" s="113"/>
+    </row>
+    <row r="18" spans="1:17" ht="9">
       <c r="A18" s="19" t="s">
         <v>50</v>
       </c>
@@ -2482,8 +2531,9 @@
       <c r="P18" s="12">
         <v>356537</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" ht="9">
+      <c r="Q18" s="113"/>
+    </row>
+    <row r="19" spans="1:17" ht="9">
       <c r="A19" s="19" t="s">
         <v>49</v>
       </c>
@@ -2532,8 +2582,9 @@
       <c r="P19" s="20">
         <v>18464506</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" ht="9">
+      <c r="Q19" s="113"/>
+    </row>
+    <row r="20" spans="1:17" ht="9">
       <c r="A20" s="19" t="s">
         <v>48</v>
       </c>
@@ -2582,8 +2633,9 @@
       <c r="P20" s="20">
         <v>8829596</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" ht="9">
+      <c r="Q20" s="113"/>
+    </row>
+    <row r="21" spans="1:17" ht="9">
       <c r="A21" s="19" t="s">
         <v>47</v>
       </c>
@@ -2632,8 +2684,9 @@
       <c r="P21" s="31">
         <v>1244935</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" ht="9">
+      <c r="Q21" s="113"/>
+    </row>
+    <row r="22" spans="1:17" ht="9">
       <c r="A22" s="52" t="s">
         <v>46</v>
       </c>
@@ -2682,8 +2735,9 @@
       <c r="P22" s="20">
         <v>1917677</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" ht="9">
+      <c r="Q22" s="113"/>
+    </row>
+    <row r="23" spans="1:17" ht="9">
       <c r="A23" s="19" t="s">
         <v>45</v>
       </c>
@@ -2732,8 +2786,9 @@
       <c r="P23" s="20">
         <v>10587725</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" ht="9">
+      <c r="Q23" s="113"/>
+    </row>
+    <row r="24" spans="1:17" ht="9">
       <c r="A24" s="19" t="s">
         <v>44</v>
       </c>
@@ -2782,8 +2837,9 @@
       <c r="P24" s="20">
         <v>6199901</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" ht="9">
+      <c r="Q24" s="113"/>
+    </row>
+    <row r="25" spans="1:17" ht="9">
       <c r="A25" s="43" t="s">
         <v>43</v>
       </c>
@@ -2832,8 +2888,9 @@
       <c r="P25" s="31">
         <v>3787224</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" ht="9">
+      <c r="Q25" s="113"/>
+    </row>
+    <row r="26" spans="1:17" ht="9">
       <c r="A26" s="19" t="s">
         <v>42</v>
       </c>
@@ -2882,8 +2939,9 @@
       <c r="P26" s="12">
         <v>2603543</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" ht="9">
+      <c r="Q26" s="113"/>
+    </row>
+    <row r="27" spans="1:17" ht="9">
       <c r="A27" s="19" t="s">
         <v>41</v>
       </c>
@@ -2932,8 +2990,9 @@
       <c r="P27" s="20">
         <v>4459685</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" ht="9">
+      <c r="Q27" s="113"/>
+    </row>
+    <row r="28" spans="1:17" ht="9">
       <c r="A28" s="19" t="s">
         <v>40</v>
       </c>
@@ -2982,8 +3041,9 @@
       <c r="P28" s="12">
         <v>3861204</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" ht="9">
+      <c r="Q28" s="113"/>
+    </row>
+    <row r="29" spans="1:17" ht="9">
       <c r="A29" s="19" t="s">
         <v>39</v>
       </c>
@@ -3032,8 +3092,9 @@
       <c r="P29" s="42">
         <v>1121106</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" ht="9">
+      <c r="Q29" s="113"/>
+    </row>
+    <row r="30" spans="1:17" ht="9">
       <c r="A30" s="52" t="s">
         <v>38</v>
       </c>
@@ -3082,8 +3143,9 @@
       <c r="P30" s="20">
         <v>4211377</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" ht="9">
+      <c r="Q30" s="113"/>
+    </row>
+    <row r="31" spans="1:17" ht="9">
       <c r="A31" s="19" t="s">
         <v>37</v>
       </c>
@@ -3132,8 +3194,9 @@
       <c r="P31" s="65">
         <v>5036686</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" ht="9">
+      <c r="Q31" s="113"/>
+    </row>
+    <row r="32" spans="1:17" ht="9">
       <c r="A32" s="19" t="s">
         <v>36</v>
       </c>
@@ -3182,8 +3245,9 @@
       <c r="P32" s="12">
         <v>8453239</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" ht="9">
+      <c r="Q32" s="113"/>
+    </row>
+    <row r="33" spans="1:17" ht="9">
       <c r="A33" s="43" t="s">
         <v>35</v>
       </c>
@@ -3232,8 +3296,9 @@
       <c r="P33" s="42">
         <v>5690749</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" ht="9">
+      <c r="Q33" s="113"/>
+    </row>
+    <row r="34" spans="1:17" ht="9">
       <c r="A34" s="19" t="s">
         <v>34</v>
       </c>
@@ -3282,8 +3347,9 @@
       <c r="P34" s="20">
         <v>2058975</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" ht="9">
+      <c r="Q34" s="113"/>
+    </row>
+    <row r="35" spans="1:17" ht="9">
       <c r="A35" s="19" t="s">
         <v>33</v>
       </c>
@@ -3332,8 +3398,9 @@
       <c r="P35" s="12">
         <v>5587022</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" ht="9">
+      <c r="Q35" s="113"/>
+    </row>
+    <row r="36" spans="1:17" ht="9">
       <c r="A36" s="19" t="s">
         <v>32</v>
       </c>
@@ -3382,8 +3449,9 @@
       <c r="P36" s="20">
         <v>1952553</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" ht="9">
+      <c r="Q36" s="113"/>
+    </row>
+    <row r="37" spans="1:17" ht="9">
       <c r="A37" s="19" t="s">
         <v>31</v>
       </c>
@@ -3432,8 +3500,9 @@
       <c r="P37" s="31">
         <v>1935357</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" ht="9">
+      <c r="Q37" s="113"/>
+    </row>
+    <row r="38" spans="1:17" ht="9">
       <c r="A38" s="52" t="s">
         <v>30</v>
       </c>
@@ -3482,8 +3551,9 @@
       <c r="P38" s="51">
         <v>2549357</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" ht="9">
+      <c r="Q38" s="113"/>
+    </row>
+    <row r="39" spans="1:17" ht="9">
       <c r="A39" s="19" t="s">
         <v>29</v>
       </c>
@@ -3532,8 +3602,9 @@
       <c r="P39" s="12">
         <v>1357535</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" ht="9">
+      <c r="Q39" s="113"/>
+    </row>
+    <row r="40" spans="1:17" ht="9">
       <c r="A40" s="19" t="s">
         <v>28</v>
       </c>
@@ -3582,8 +3653,9 @@
       <c r="P40" s="20">
         <v>6006247</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" ht="9">
+      <c r="Q40" s="113"/>
+    </row>
+    <row r="41" spans="1:17" ht="9">
       <c r="A41" s="43" t="s">
         <v>27</v>
       </c>
@@ -3632,8 +3704,9 @@
       <c r="P41" s="31">
         <v>1783151</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" ht="9">
+      <c r="Q41" s="113"/>
+    </row>
+    <row r="42" spans="1:17" ht="9">
       <c r="A42" s="19" t="s">
         <v>26</v>
       </c>
@@ -3682,8 +3755,9 @@
       <c r="P42" s="20">
         <v>11324755</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" ht="9">
+      <c r="Q42" s="113"/>
+    </row>
+    <row r="43" spans="1:17" ht="9">
       <c r="A43" s="19" t="s">
         <v>25</v>
       </c>
@@ -3732,8 +3806,9 @@
       <c r="P43" s="20">
         <v>8739280</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" ht="9">
+      <c r="Q43" s="113"/>
+    </row>
+    <row r="44" spans="1:17" ht="9">
       <c r="A44" s="19" t="s">
         <v>24</v>
       </c>
@@ -3782,8 +3857,9 @@
       <c r="P44" s="20">
         <v>899083</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" ht="9">
+      <c r="Q44" s="113"/>
+    </row>
+    <row r="45" spans="1:17" ht="9">
       <c r="A45" s="19" t="s">
         <v>23</v>
       </c>
@@ -3832,8 +3908,9 @@
       <c r="P45" s="31">
         <v>10592317</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" ht="9">
+      <c r="Q45" s="113"/>
+    </row>
+    <row r="46" spans="1:17" ht="9">
       <c r="A46" s="52" t="s">
         <v>22</v>
       </c>
@@ -3882,8 +3959,9 @@
       <c r="P46" s="20">
         <v>3730247</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" ht="9">
+      <c r="Q46" s="113"/>
+    </row>
+    <row r="47" spans="1:17" ht="9">
       <c r="A47" s="19" t="s">
         <v>21</v>
       </c>
@@ -3932,8 +4010,9 @@
       <c r="P47" s="20">
         <v>4095442</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" ht="9">
+      <c r="Q47" s="113"/>
+    </row>
+    <row r="48" spans="1:17" ht="9">
       <c r="A48" s="19" t="s">
         <v>20</v>
       </c>
@@ -3982,8 +4061,9 @@
       <c r="P48" s="20">
         <v>10690187</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" ht="9">
+      <c r="Q48" s="113"/>
+    </row>
+    <row r="49" spans="1:17" ht="9">
       <c r="A49" s="43" t="s">
         <v>19</v>
       </c>
@@ -4032,8 +4112,9 @@
       <c r="P49" s="31">
         <v>866625</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" ht="9">
+      <c r="Q49" s="113"/>
+    </row>
+    <row r="50" spans="1:17" ht="9">
       <c r="A50" s="19" t="s">
         <v>18</v>
       </c>
@@ -4082,8 +4163,9 @@
       <c r="P50" s="20">
         <v>4561299</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" ht="9">
+      <c r="Q50" s="113"/>
+    </row>
+    <row r="51" spans="1:17" ht="9">
       <c r="A51" s="19" t="s">
         <v>17</v>
       </c>
@@ -4132,8 +4214,9 @@
       <c r="P51" s="12">
         <v>1294282</v>
       </c>
-    </row>
-    <row r="52" spans="1:16" ht="9">
+      <c r="Q51" s="113"/>
+    </row>
+    <row r="52" spans="1:17" ht="9">
       <c r="A52" s="19" t="s">
         <v>16</v>
       </c>
@@ -4182,8 +4265,9 @@
       <c r="P52" s="20">
         <v>5855373</v>
       </c>
-    </row>
-    <row r="53" spans="1:16" ht="9">
+      <c r="Q52" s="113"/>
+    </row>
+    <row r="53" spans="1:17" ht="9">
       <c r="A53" s="19" t="s">
         <v>15</v>
       </c>
@@ -4232,8 +4316,9 @@
       <c r="P53" s="31">
         <v>22419490</v>
       </c>
-    </row>
-    <row r="54" spans="1:16" ht="9">
+      <c r="Q53" s="113"/>
+    </row>
+    <row r="54" spans="1:17" ht="9">
       <c r="A54" s="52" t="s">
         <v>14</v>
       </c>
@@ -4282,8 +4367,9 @@
       <c r="P54" s="20">
         <v>2479604</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" ht="9">
+      <c r="Q54" s="113"/>
+    </row>
+    <row r="55" spans="1:17" ht="9">
       <c r="A55" s="19" t="s">
         <v>13</v>
       </c>
@@ -4332,8 +4418,9 @@
       <c r="P55" s="20">
         <v>607890</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" ht="9">
+      <c r="Q55" s="113"/>
+    </row>
+    <row r="56" spans="1:17" ht="9">
       <c r="A56" s="19" t="s">
         <v>12</v>
       </c>
@@ -4382,8 +4469,9 @@
       <c r="P56" s="20">
         <v>7606452</v>
       </c>
-    </row>
-    <row r="57" spans="1:16" ht="9">
+      <c r="Q56" s="113"/>
+    </row>
+    <row r="57" spans="1:17" ht="9">
       <c r="A57" s="43" t="s">
         <v>11</v>
       </c>
@@ -4432,8 +4520,9 @@
       <c r="P57" s="31">
         <v>7257401</v>
       </c>
-    </row>
-    <row r="58" spans="1:16" ht="9">
+      <c r="Q57" s="113"/>
+    </row>
+    <row r="58" spans="1:17" ht="9">
       <c r="A58" s="19" t="s">
         <v>10</v>
       </c>
@@ -4482,8 +4571,9 @@
       <c r="P58" s="12">
         <v>1657362</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" ht="9">
+      <c r="Q58" s="113"/>
+    </row>
+    <row r="59" spans="1:17" ht="9">
       <c r="A59" s="19" t="s">
         <v>9</v>
       </c>
@@ -4532,8 +4622,9 @@
       <c r="P59" s="20">
         <v>5616271</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" ht="9">
+      <c r="Q59" s="113"/>
+    </row>
+    <row r="60" spans="1:17" ht="9">
       <c r="A60" s="19" t="s">
         <v>8</v>
       </c>
@@ -4582,8 +4673,9 @@
       <c r="P60" s="12">
         <v>861028</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" ht="9">
+      <c r="Q60" s="113"/>
+    </row>
+    <row r="61" spans="1:17" ht="9">
       <c r="A61" s="11" t="s">
         <v>7</v>
       </c>
@@ -4633,7 +4725,7 @@
         <v>275913237</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="9">
+    <row r="62" spans="1:17" ht="9">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -4651,7 +4743,7 @@
       <c r="O62" s="5"/>
       <c r="P62" s="5"/>
     </row>
-    <row r="63" spans="1:16" ht="39.6" customHeight="1">
+    <row r="63" spans="1:17" ht="39.65" customHeight="1">
       <c r="A63" s="104" t="s">
         <v>6</v>
       </c>
@@ -4683,32 +4775,32 @@
     <mergeCell ref="N5:P5"/>
   </mergeCells>
   <conditionalFormatting sqref="B28">
-    <cfRule type="cellIs" dxfId="5" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="34" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:D27">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:D60">
-    <cfRule type="cellIs" dxfId="3" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:E10 E11:E62">
-    <cfRule type="cellIs" dxfId="2" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="25" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:D29">
-    <cfRule type="cellIs" dxfId="1" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="21" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:P60">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4724,37 +4816,37 @@
   </sheetPr>
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="7" width="13.7109375" customWidth="1"/>
+    <col min="2" max="7" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="99" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>79</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>80</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>81</v>
-      </c>
-      <c r="G1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -4991,7 +5083,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10">
         <f>'Table MV-1'!D18/'Table MV-1'!$D$61</f>
@@ -5368,7 +5460,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B23">
         <f>'Table MV-1'!D31/'Table MV-1'!$D$61</f>
@@ -6238,7 +6330,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -6261,7 +6353,7 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -6284,7 +6376,7 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -6307,7 +6399,7 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -6330,7 +6422,7 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -6353,7 +6445,7 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -6376,7 +6468,7 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -6399,7 +6491,7 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -6422,7 +6514,7 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -6460,33 +6552,33 @@
       <selection activeCell="D2" sqref="D2:F52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="7" width="13.7109375" customWidth="1"/>
+    <col min="2" max="7" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="99" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>79</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>80</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>81</v>
-      </c>
-      <c r="G1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -6715,7 +6807,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
@@ -7079,7 +7171,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
@@ -7919,7 +8011,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -7942,7 +8034,7 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -7965,7 +8057,7 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -7988,7 +8080,7 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -8011,7 +8103,7 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -8034,7 +8126,7 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -8057,7 +8149,7 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -8080,7 +8172,7 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -8103,7 +8195,7 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B61">
         <v>0</v>

</xml_diff>